<commit_message>
Make both total scores bolded in template spreadsheet
</commit_message>
<xml_diff>
--- a/DeepSpace Scoring Optimizer.xlsx
+++ b/DeepSpace Scoring Optimizer.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21519"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A8B3C15-4571-42F9-A81F-E6DE1AD47214}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5940F6E2-6D5A-425E-BF17-ED67123BD015}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,13 +119,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -270,10 +263,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -282,7 +275,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -291,16 +288,13 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -315,7 +309,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +626,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -656,10 +649,10 @@
       <c r="B2"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
@@ -686,142 +679,142 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1">
-      <c r="A5" s="17"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1"/>
     <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="12" t="s">
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="C12" s="11"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:12" ht="11.25" customHeight="1">
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>